<commit_message>
update my_bets and probables
</commit_message>
<xml_diff>
--- a/swertres/my_bets_excel.xlsx
+++ b/swertres/my_bets_excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>DATE - TIME</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>03 mon jun 2019 1</t>
+  </si>
+  <si>
+    <t>04 tue jun 2019 0</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,6 +450,41 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>240</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>244</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>246</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>224</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>